<commit_message>
Added new rollup type for first order by
</commit_message>
<xml_diff>
--- a/Customisations/Test Customisations Calculations.xlsx
+++ b/Customisations/Test Customisations Calculations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="125">
   <si>
     <t>Display Name</t>
   </si>
@@ -226,6 +226,12 @@
     <t>Boolean</t>
   </si>
   <si>
+    <t>jmcg_firsttarget</t>
+  </si>
+  <si>
+    <t>jmcg_firsttargettestentitytwo</t>
+  </si>
+  <si>
     <t>jmcg_testentitytwo</t>
   </si>
   <si>
@@ -287,6 +293,12 @@
   </si>
   <si>
     <t>String</t>
+  </si>
+  <si>
+    <t>jmcg_firstsource</t>
+  </si>
+  <si>
+    <t>jmcg_firstsourceorderby</t>
   </si>
   <si>
     <t>jmcg_testentityrollupreference</t>
@@ -9105,19 +9117,19 @@
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="C24" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>42</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F24" s="2" t="b">
         <v>0</v>
@@ -9167,19 +9179,19 @@
     </row>
     <row r="25">
       <c r="A25" s="3" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>44</v>
+        <v>71</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F25" s="2" t="b">
         <v>0</v>
@@ -9194,10 +9206,14 @@
         <v>0</v>
       </c>
       <c r="J25" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
+        <v>3.0</v>
+      </c>
+      <c r="K25" s="2">
+        <v>150.0</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="M25" s="2" t="b">
         <v>0</v>
       </c>
@@ -9227,7 +9243,7 @@
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>73</v>
@@ -9236,7 +9252,7 @@
         <v>73</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>73</v>
@@ -9254,9 +9270,11 @@
         <v>0</v>
       </c>
       <c r="J26" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="K26" s="2"/>
+        <v>3.0</v>
+      </c>
+      <c r="K26" s="2">
+        <v>150.0</v>
+      </c>
       <c r="L26" s="2"/>
       <c r="M26" s="2" t="b">
         <v>0</v>
@@ -9287,7 +9305,7 @@
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>74</v>
@@ -9296,7 +9314,7 @@
         <v>74</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>74</v>
@@ -9313,7 +9331,9 @@
       <c r="I27" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J27" s="2"/>
+      <c r="J27" s="2">
+        <v>4.0</v>
+      </c>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2" t="b">
@@ -9345,7 +9365,7 @@
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>75</v>
@@ -9354,7 +9374,7 @@
         <v>75</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>75</v>
@@ -9372,11 +9392,9 @@
         <v>0</v>
       </c>
       <c r="J28" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="K28" s="2">
-        <v>150.0</v>
-      </c>
+        <v>4.0</v>
+      </c>
+      <c r="K28" s="2"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2" t="b">
         <v>0</v>
@@ -9407,7 +9425,7 @@
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>76</v>
@@ -9416,7 +9434,7 @@
         <v>76</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>76</v>
@@ -9433,9 +9451,7 @@
       <c r="I29" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J29" s="2">
-        <v>4.0</v>
-      </c>
+      <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2" t="b">
@@ -9467,7 +9483,7 @@
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>77</v>
@@ -9476,7 +9492,7 @@
         <v>77</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>77</v>
@@ -9494,9 +9510,11 @@
         <v>0</v>
       </c>
       <c r="J30" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="K30" s="2"/>
+        <v>3.0</v>
+      </c>
+      <c r="K30" s="2">
+        <v>150.0</v>
+      </c>
       <c r="L30" s="2"/>
       <c r="M30" s="2" t="b">
         <v>0</v>
@@ -9527,7 +9545,7 @@
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>78</v>
@@ -9536,7 +9554,7 @@
         <v>78</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>78</v>
@@ -9553,7 +9571,9 @@
       <c r="I31" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J31" s="2"/>
+      <c r="J31" s="2">
+        <v>4.0</v>
+      </c>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2" t="b">
@@ -9585,7 +9605,7 @@
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>79</v>
@@ -9594,7 +9614,7 @@
         <v>79</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>79</v>
@@ -9611,7 +9631,9 @@
       <c r="I32" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J32" s="2"/>
+      <c r="J32" s="2">
+        <v>4.0</v>
+      </c>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2" t="b">
@@ -9620,14 +9642,14 @@
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
-      <c r="Q32" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="R32" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="S32" s="2"/>
-      <c r="T32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T32" s="2">
+        <v>100000.0</v>
+      </c>
       <c r="U32" s="1">
         <v>4.0</v>
       </c>
@@ -9643,7 +9665,7 @@
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>80</v>
@@ -9652,7 +9674,7 @@
         <v>80</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>80</v>
@@ -9669,12 +9691,8 @@
       <c r="I33" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J33" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="K33" s="2">
-        <v>150.0</v>
-      </c>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2" t="b">
         <v>0</v>
@@ -9705,7 +9723,7 @@
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>81</v>
@@ -9714,7 +9732,7 @@
         <v>81</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>81</v>
@@ -9731,9 +9749,7 @@
       <c r="I34" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J34" s="2">
-        <v>4.0</v>
-      </c>
+      <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2" t="b">
@@ -9742,14 +9758,14 @@
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
-      <c r="Q34" s="2"/>
-      <c r="R34" s="2"/>
-      <c r="S34" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="T34" s="2">
-        <v>100000.0</v>
-      </c>
+      <c r="Q34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="R34" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
       <c r="U34" s="1">
         <v>4.0</v>
       </c>
@@ -9765,7 +9781,7 @@
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>82</v>
@@ -9774,7 +9790,7 @@
         <v>82</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>82</v>
@@ -9792,9 +9808,11 @@
         <v>0</v>
       </c>
       <c r="J35" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="K35" s="2"/>
+        <v>3.0</v>
+      </c>
+      <c r="K35" s="2">
+        <v>150.0</v>
+      </c>
       <c r="L35" s="2"/>
       <c r="M35" s="2" t="b">
         <v>0</v>
@@ -9825,7 +9843,7 @@
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>83</v>
@@ -9834,7 +9852,7 @@
         <v>83</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>83</v>
@@ -9851,7 +9869,9 @@
       <c r="I36" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J36" s="2"/>
+      <c r="J36" s="2">
+        <v>4.0</v>
+      </c>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2" t="b">
@@ -9883,7 +9903,7 @@
     </row>
     <row r="37">
       <c r="A37" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>84</v>
@@ -9892,7 +9912,7 @@
         <v>84</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>84</v>
@@ -9909,7 +9929,9 @@
       <c r="I37" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J37" s="2"/>
+      <c r="J37" s="2">
+        <v>4.0</v>
+      </c>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2" t="b">
@@ -9918,14 +9940,14 @@
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
-      <c r="Q37" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="R37" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="S37" s="2"/>
-      <c r="T37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T37" s="2">
+        <v>100000.0</v>
+      </c>
       <c r="U37" s="1">
         <v>4.0</v>
       </c>
@@ -9941,7 +9963,7 @@
     </row>
     <row r="38">
       <c r="A38" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>85</v>
@@ -9950,7 +9972,7 @@
         <v>85</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>85</v>
@@ -9967,12 +9989,8 @@
       <c r="I38" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J38" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="K38" s="2">
-        <v>150.0</v>
-      </c>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2" t="b">
         <v>0</v>
@@ -10003,7 +10021,7 @@
     </row>
     <row r="39">
       <c r="A39" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>86</v>
@@ -10012,7 +10030,7 @@
         <v>86</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>86</v>
@@ -10029,9 +10047,7 @@
       <c r="I39" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J39" s="2">
-        <v>4.0</v>
-      </c>
+      <c r="J39" s="2"/>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2" t="b">
@@ -10040,14 +10056,14 @@
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="R39" s="2"/>
-      <c r="S39" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="T39" s="2">
-        <v>100000.0</v>
-      </c>
+      <c r="Q39" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="R39" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
       <c r="U39" s="1">
         <v>4.0</v>
       </c>
@@ -10063,7 +10079,7 @@
     </row>
     <row r="40">
       <c r="A40" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>87</v>
@@ -10072,7 +10088,7 @@
         <v>87</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>87</v>
@@ -10090,9 +10106,11 @@
         <v>0</v>
       </c>
       <c r="J40" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="K40" s="2"/>
+        <v>3.0</v>
+      </c>
+      <c r="K40" s="2">
+        <v>150.0</v>
+      </c>
       <c r="L40" s="2"/>
       <c r="M40" s="2" t="b">
         <v>0</v>
@@ -10123,7 +10141,7 @@
     </row>
     <row r="41">
       <c r="A41" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>88</v>
@@ -10132,7 +10150,7 @@
         <v>88</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>88</v>
@@ -10149,7 +10167,9 @@
       <c r="I41" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J41" s="2"/>
+      <c r="J41" s="2">
+        <v>4.0</v>
+      </c>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
       <c r="M41" s="2" t="b">
@@ -10181,7 +10201,7 @@
     </row>
     <row r="42">
       <c r="A42" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>89</v>
@@ -10190,7 +10210,7 @@
         <v>89</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>89</v>
@@ -10208,24 +10228,24 @@
         <v>0</v>
       </c>
       <c r="J42" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="K42" s="2">
-        <v>100.0</v>
-      </c>
+        <v>4.0</v>
+      </c>
+      <c r="K42" s="2"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="N42" s="2">
-        <v>200.0</v>
-      </c>
+      <c r="N42" s="2"/>
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
-      <c r="S42" s="2"/>
-      <c r="T42" s="2"/>
+      <c r="S42" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T42" s="2">
+        <v>100000.0</v>
+      </c>
       <c r="U42" s="1">
         <v>4.0</v>
       </c>
@@ -10241,19 +10261,19 @@
     </row>
     <row r="43">
       <c r="A43" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F43" s="2" t="b">
         <v>0</v>
@@ -10269,9 +10289,7 @@
       </c>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
-      <c r="L43" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="L43" s="2"/>
       <c r="M43" s="2" t="b">
         <v>0</v>
       </c>
@@ -10280,8 +10298,12 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
-      <c r="S43" s="2"/>
-      <c r="T43" s="2"/>
+      <c r="S43" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T43" s="2">
+        <v>100000.0</v>
+      </c>
       <c r="U43" s="1">
         <v>4.0</v>
       </c>
@@ -10295,110 +10317,230 @@
       <c r="AA43" s="2"/>
       <c r="AB43" s="2"/>
     </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
+    <row r="44">
+      <c r="A44" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F44" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H44" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J44" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="K44" s="2">
+        <v>100.0</v>
+      </c>
       <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
+      <c r="M44" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N44" s="2">
+        <v>200.0</v>
+      </c>
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
-      <c r="U44" s="2"/>
+      <c r="U44" s="1">
+        <v>4.0</v>
+      </c>
       <c r="V44" s="2"/>
-      <c r="W44" s="2"/>
+      <c r="W44" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="X44" s="2"/>
       <c r="Y44" s="2"/>
       <c r="Z44" s="2"/>
       <c r="AA44" s="2"/>
       <c r="AB44" s="2"/>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
+    <row r="45">
+      <c r="A45" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F45" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H45" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I45" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J45" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="K45" s="2">
+        <v>100.0</v>
+      </c>
       <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
+      <c r="M45" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N45" s="2">
+        <v>200.0</v>
+      </c>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
-      <c r="S45" s="2"/>
-      <c r="T45" s="2"/>
-      <c r="U45" s="2"/>
+      <c r="S45" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T45" s="2">
+        <v>100000.0</v>
+      </c>
+      <c r="U45" s="1">
+        <v>4.0</v>
+      </c>
       <c r="V45" s="2"/>
-      <c r="W45" s="2"/>
+      <c r="W45" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="X45" s="2"/>
       <c r="Y45" s="2"/>
       <c r="Z45" s="2"/>
       <c r="AA45" s="2"/>
       <c r="AB45" s="2"/>
     </row>
-    <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
+    <row r="46">
+      <c r="A46" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F46" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G46" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H46" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I46" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J46" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="K46" s="2">
+        <v>100.0</v>
+      </c>
       <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
+      <c r="M46" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N46" s="2">
+        <v>200.0</v>
+      </c>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
-      <c r="S46" s="2"/>
-      <c r="T46" s="2"/>
-      <c r="U46" s="2"/>
+      <c r="S46" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T46" s="2">
+        <v>100000.0</v>
+      </c>
+      <c r="U46" s="1">
+        <v>4.0</v>
+      </c>
       <c r="V46" s="2"/>
-      <c r="W46" s="2"/>
+      <c r="W46" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="X46" s="2"/>
       <c r="Y46" s="2"/>
       <c r="Z46" s="2"/>
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
     </row>
-    <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
+    <row r="47">
+      <c r="A47" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F47" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H47" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
+      <c r="L47" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M47" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
@@ -10406,9 +10548,13 @@
       <c r="R47" s="2"/>
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
-      <c r="U47" s="2"/>
+      <c r="U47" s="1">
+        <v>4.0</v>
+      </c>
       <c r="V47" s="2"/>
-      <c r="W47" s="2"/>
+      <c r="W47" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="X47" s="2"/>
       <c r="Y47" s="2"/>
       <c r="Z47" s="2"/>
@@ -15156,28 +15302,124 @@
       <c r="AB205" s="2"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="D206" s="4"/>
-      <c r="O206" s="4"/>
+      <c r="A206" s="2"/>
+      <c r="B206" s="2"/>
+      <c r="C206" s="2"/>
+      <c r="D206" s="2"/>
+      <c r="E206" s="2"/>
+      <c r="F206" s="2"/>
+      <c r="G206" s="2"/>
+      <c r="H206" s="2"/>
+      <c r="I206" s="2"/>
+      <c r="J206" s="2"/>
+      <c r="K206" s="2"/>
+      <c r="L206" s="2"/>
+      <c r="M206" s="2"/>
+      <c r="N206" s="2"/>
+      <c r="O206" s="2"/>
       <c r="P206" s="2"/>
-      <c r="Q206" s="4"/>
+      <c r="Q206" s="2"/>
+      <c r="R206" s="2"/>
+      <c r="S206" s="2"/>
+      <c r="T206" s="2"/>
+      <c r="U206" s="2"/>
+      <c r="V206" s="2"/>
+      <c r="W206" s="2"/>
+      <c r="X206" s="2"/>
+      <c r="Y206" s="2"/>
+      <c r="Z206" s="2"/>
+      <c r="AA206" s="2"/>
+      <c r="AB206" s="2"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="D207" s="4"/>
-      <c r="O207" s="4"/>
+      <c r="A207" s="2"/>
+      <c r="B207" s="2"/>
+      <c r="C207" s="2"/>
+      <c r="D207" s="2"/>
+      <c r="E207" s="2"/>
+      <c r="F207" s="2"/>
+      <c r="G207" s="2"/>
+      <c r="H207" s="2"/>
+      <c r="I207" s="2"/>
+      <c r="J207" s="2"/>
+      <c r="K207" s="2"/>
+      <c r="L207" s="2"/>
+      <c r="M207" s="2"/>
+      <c r="N207" s="2"/>
+      <c r="O207" s="2"/>
       <c r="P207" s="2"/>
-      <c r="Q207" s="4"/>
+      <c r="Q207" s="2"/>
+      <c r="R207" s="2"/>
+      <c r="S207" s="2"/>
+      <c r="T207" s="2"/>
+      <c r="U207" s="2"/>
+      <c r="V207" s="2"/>
+      <c r="W207" s="2"/>
+      <c r="X207" s="2"/>
+      <c r="Y207" s="2"/>
+      <c r="Z207" s="2"/>
+      <c r="AA207" s="2"/>
+      <c r="AB207" s="2"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="D208" s="4"/>
-      <c r="O208" s="4"/>
+      <c r="A208" s="2"/>
+      <c r="B208" s="2"/>
+      <c r="C208" s="2"/>
+      <c r="D208" s="2"/>
+      <c r="E208" s="2"/>
+      <c r="F208" s="2"/>
+      <c r="G208" s="2"/>
+      <c r="H208" s="2"/>
+      <c r="I208" s="2"/>
+      <c r="J208" s="2"/>
+      <c r="K208" s="2"/>
+      <c r="L208" s="2"/>
+      <c r="M208" s="2"/>
+      <c r="N208" s="2"/>
+      <c r="O208" s="2"/>
       <c r="P208" s="2"/>
-      <c r="Q208" s="4"/>
+      <c r="Q208" s="2"/>
+      <c r="R208" s="2"/>
+      <c r="S208" s="2"/>
+      <c r="T208" s="2"/>
+      <c r="U208" s="2"/>
+      <c r="V208" s="2"/>
+      <c r="W208" s="2"/>
+      <c r="X208" s="2"/>
+      <c r="Y208" s="2"/>
+      <c r="Z208" s="2"/>
+      <c r="AA208" s="2"/>
+      <c r="AB208" s="2"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="D209" s="4"/>
-      <c r="O209" s="4"/>
+      <c r="A209" s="2"/>
+      <c r="B209" s="2"/>
+      <c r="C209" s="2"/>
+      <c r="D209" s="2"/>
+      <c r="E209" s="2"/>
+      <c r="F209" s="2"/>
+      <c r="G209" s="2"/>
+      <c r="H209" s="2"/>
+      <c r="I209" s="2"/>
+      <c r="J209" s="2"/>
+      <c r="K209" s="2"/>
+      <c r="L209" s="2"/>
+      <c r="M209" s="2"/>
+      <c r="N209" s="2"/>
+      <c r="O209" s="2"/>
       <c r="P209" s="2"/>
-      <c r="Q209" s="4"/>
+      <c r="Q209" s="2"/>
+      <c r="R209" s="2"/>
+      <c r="S209" s="2"/>
+      <c r="T209" s="2"/>
+      <c r="U209" s="2"/>
+      <c r="V209" s="2"/>
+      <c r="W209" s="2"/>
+      <c r="X209" s="2"/>
+      <c r="Y209" s="2"/>
+      <c r="Z209" s="2"/>
+      <c r="AA209" s="2"/>
+      <c r="AB209" s="2"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
       <c r="D210" s="4"/>
@@ -19793,18 +20035,42 @@
       <c r="P978" s="2"/>
       <c r="Q978" s="4"/>
     </row>
+    <row r="979" ht="15.75" customHeight="1">
+      <c r="D979" s="4"/>
+      <c r="O979" s="4"/>
+      <c r="P979" s="2"/>
+      <c r="Q979" s="4"/>
+    </row>
+    <row r="980" ht="15.75" customHeight="1">
+      <c r="D980" s="4"/>
+      <c r="O980" s="4"/>
+      <c r="P980" s="2"/>
+      <c r="Q980" s="4"/>
+    </row>
+    <row r="981" ht="15.75" customHeight="1">
+      <c r="D981" s="4"/>
+      <c r="O981" s="4"/>
+      <c r="P981" s="2"/>
+      <c r="Q981" s="4"/>
+    </row>
+    <row r="982" ht="15.75" customHeight="1">
+      <c r="D982" s="4"/>
+      <c r="O982" s="4"/>
+      <c r="P982" s="2"/>
+      <c r="Q982" s="4"/>
+    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="Q2:Q978">
+    <dataValidation type="list" allowBlank="1" sqref="Q2:Q982">
       <formula1>"UserLocal,DateOnly,TimeZoneIndependent"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="O2:O978">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="O2:O982">
       <formula1>"Text,TextArea,Email,Url,TickerSymbol,Phone"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="D2:D978">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="D2:D982">
       <formula1>"Boolean,Date,Decimal,Double,Integer,Lookup,Money,Picklist,String,Memo,Status"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="P2:P978">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="P2:P982">
       <formula1>"None,Duration,Language,TimeZone"</formula1>
     </dataValidation>
   </dataValidations>
@@ -19840,16 +20106,16 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="2"/>
@@ -19875,7 +20141,7 @@
     <row r="2">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>0</v>
@@ -19884,7 +20150,7 @@
         <v>1.0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -19910,7 +20176,7 @@
     <row r="3">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>0</v>
@@ -19919,7 +20185,7 @@
         <v>2.0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -19944,10 +20210,10 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
@@ -19956,7 +20222,7 @@
         <v>1.0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -19981,10 +20247,10 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
@@ -19993,7 +20259,7 @@
         <v>2.0</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -20019,7 +20285,7 @@
     <row r="6">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>0</v>
@@ -20028,7 +20294,7 @@
         <v>1.0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -20055,7 +20321,7 @@
     <row r="7">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>0</v>
@@ -20064,7 +20330,7 @@
         <v>2.0</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -26649,37 +26915,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -26699,7 +26965,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>12</v>
@@ -26720,16 +26986,16 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="J2" s="2">
         <v>15000.0</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -26749,7 +27015,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
@@ -26770,13 +27036,13 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="K3" s="2">
         <v>20000.0</v>

</xml_diff>

<commit_message>
Added calculation type add time
</commit_message>
<xml_diff>
--- a/Customisations/Test Customisations Calculations.xlsx
+++ b/Customisations/Test Customisations Calculations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="133">
   <si>
     <t>Display Name</t>
   </si>
@@ -233,6 +233,30 @@
   </si>
   <si>
     <t>jmcg_testentitytwo</t>
+  </si>
+  <si>
+    <t>jmcg_dateaddtoutc</t>
+  </si>
+  <si>
+    <t>jmcg_dateaddresultutc</t>
+  </si>
+  <si>
+    <t>jmcg_dateaddtodateonly</t>
+  </si>
+  <si>
+    <t>DateOnly</t>
+  </si>
+  <si>
+    <t>jmcg_dateaddresultdateonly</t>
+  </si>
+  <si>
+    <t>jmcg_dateaddtonotimezone</t>
+  </si>
+  <si>
+    <t>TimeZoneIndependent</t>
+  </si>
+  <si>
+    <t>jmcg_dateaddresultnotimezone</t>
   </si>
   <si>
     <t>jmcg_integersumsource</t>
@@ -9243,7 +9267,7 @@
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>73</v>
@@ -9251,8 +9275,8 @@
       <c r="C26" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>42</v>
+      <c r="D26" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>73</v>
@@ -9282,7 +9306,9 @@
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
-      <c r="Q26" s="2"/>
+      <c r="Q26" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="R26" s="2"/>
       <c r="S26" s="2">
         <v>0.0</v>
@@ -9305,7 +9331,7 @@
     </row>
     <row r="27">
       <c r="A27" s="3" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>74</v>
@@ -9313,8 +9339,8 @@
       <c r="C27" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>44</v>
+      <c r="D27" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>74</v>
@@ -9332,9 +9358,11 @@
         <v>0</v>
       </c>
       <c r="J27" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="K27" s="2"/>
+        <v>3.0</v>
+      </c>
+      <c r="K27" s="2">
+        <v>150.0</v>
+      </c>
       <c r="L27" s="2"/>
       <c r="M27" s="2" t="b">
         <v>0</v>
@@ -9342,7 +9370,9 @@
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
+      <c r="Q27" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="R27" s="2"/>
       <c r="S27" s="2">
         <v>0.0</v>
@@ -9365,7 +9395,7 @@
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>75</v>
@@ -9373,8 +9403,8 @@
       <c r="C28" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>46</v>
+      <c r="D28" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>75</v>
@@ -9392,9 +9422,11 @@
         <v>0</v>
       </c>
       <c r="J28" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="K28" s="2"/>
+        <v>3.0</v>
+      </c>
+      <c r="K28" s="2">
+        <v>150.0</v>
+      </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2" t="b">
         <v>0</v>
@@ -9402,7 +9434,9 @@
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
+      <c r="Q28" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="R28" s="2"/>
       <c r="S28" s="2">
         <v>0.0</v>
@@ -9425,19 +9459,19 @@
     </row>
     <row r="29">
       <c r="A29" s="3" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>48</v>
+        <v>77</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F29" s="2" t="b">
         <v>0</v>
@@ -9451,8 +9485,12 @@
       <c r="I29" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
+      <c r="J29" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="K29" s="2">
+        <v>150.0</v>
+      </c>
       <c r="L29" s="2"/>
       <c r="M29" s="2" t="b">
         <v>0</v>
@@ -9460,7 +9498,9 @@
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
+      <c r="Q29" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="R29" s="2"/>
       <c r="S29" s="2">
         <v>0.0</v>
@@ -9483,19 +9523,19 @@
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>42</v>
+        <v>78</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F30" s="2" t="b">
         <v>0</v>
@@ -9522,7 +9562,9 @@
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
+      <c r="Q30" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="R30" s="2"/>
       <c r="S30" s="2">
         <v>0.0</v>
@@ -9545,19 +9587,19 @@
     </row>
     <row r="31">
       <c r="A31" s="3" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>44</v>
+        <v>80</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F31" s="2" t="b">
         <v>0</v>
@@ -9572,9 +9614,11 @@
         <v>0</v>
       </c>
       <c r="J31" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="K31" s="2"/>
+        <v>3.0</v>
+      </c>
+      <c r="K31" s="2">
+        <v>150.0</v>
+      </c>
       <c r="L31" s="2"/>
       <c r="M31" s="2" t="b">
         <v>0</v>
@@ -9582,7 +9626,9 @@
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
+      <c r="Q31" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="R31" s="2"/>
       <c r="S31" s="2">
         <v>0.0</v>
@@ -9608,16 +9654,16 @@
         <v>72</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F32" s="2" t="b">
         <v>0</v>
@@ -9632,9 +9678,11 @@
         <v>0</v>
       </c>
       <c r="J32" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="K32" s="2"/>
+        <v>3.0</v>
+      </c>
+      <c r="K32" s="2">
+        <v>150.0</v>
+      </c>
       <c r="L32" s="2"/>
       <c r="M32" s="2" t="b">
         <v>0</v>
@@ -9668,16 +9716,16 @@
         <v>72</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F33" s="2" t="b">
         <v>0</v>
@@ -9691,7 +9739,9 @@
       <c r="I33" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J33" s="2"/>
+      <c r="J33" s="2">
+        <v>4.0</v>
+      </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2" t="b">
@@ -9726,16 +9776,16 @@
         <v>72</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F34" s="2" t="b">
         <v>0</v>
@@ -9749,7 +9799,9 @@
       <c r="I34" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J34" s="2"/>
+      <c r="J34" s="2">
+        <v>4.0</v>
+      </c>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2" t="b">
@@ -9758,14 +9810,14 @@
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
-      <c r="Q34" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="R34" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="S34" s="2"/>
-      <c r="T34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T34" s="2">
+        <v>100000.0</v>
+      </c>
       <c r="U34" s="1">
         <v>4.0</v>
       </c>
@@ -9784,16 +9836,16 @@
         <v>72</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F35" s="2" t="b">
         <v>0</v>
@@ -9807,12 +9859,8 @@
       <c r="I35" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J35" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="K35" s="2">
-        <v>150.0</v>
-      </c>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2" t="b">
         <v>0</v>
@@ -9846,16 +9894,16 @@
         <v>72</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F36" s="2" t="b">
         <v>0</v>
@@ -9870,9 +9918,11 @@
         <v>0</v>
       </c>
       <c r="J36" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="K36" s="2"/>
+        <v>3.0</v>
+      </c>
+      <c r="K36" s="2">
+        <v>150.0</v>
+      </c>
       <c r="L36" s="2"/>
       <c r="M36" s="2" t="b">
         <v>0</v>
@@ -9906,16 +9956,16 @@
         <v>72</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F37" s="2" t="b">
         <v>0</v>
@@ -9966,16 +10016,16 @@
         <v>72</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F38" s="2" t="b">
         <v>0</v>
@@ -9989,7 +10039,9 @@
       <c r="I38" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J38" s="2"/>
+      <c r="J38" s="2">
+        <v>4.0</v>
+      </c>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2" t="b">
@@ -10024,16 +10076,16 @@
         <v>72</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F39" s="2" t="b">
         <v>0</v>
@@ -10056,14 +10108,14 @@
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
-      <c r="Q39" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="R39" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="S39" s="2"/>
-      <c r="T39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T39" s="2">
+        <v>100000.0</v>
+      </c>
       <c r="U39" s="1">
         <v>4.0</v>
       </c>
@@ -10082,16 +10134,16 @@
         <v>72</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F40" s="2" t="b">
         <v>0</v>
@@ -10105,12 +10157,8 @@
       <c r="I40" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J40" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="K40" s="2">
-        <v>150.0</v>
-      </c>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2" t="b">
         <v>0</v>
@@ -10118,14 +10166,14 @@
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="2"/>
-      <c r="S40" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="T40" s="2">
-        <v>100000.0</v>
-      </c>
+      <c r="Q40" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="R40" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
       <c r="U40" s="1">
         <v>4.0</v>
       </c>
@@ -10144,16 +10192,16 @@
         <v>72</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F41" s="2" t="b">
         <v>0</v>
@@ -10168,9 +10216,11 @@
         <v>0</v>
       </c>
       <c r="J41" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="K41" s="2"/>
+        <v>3.0</v>
+      </c>
+      <c r="K41" s="2">
+        <v>150.0</v>
+      </c>
       <c r="L41" s="2"/>
       <c r="M41" s="2" t="b">
         <v>0</v>
@@ -10204,16 +10254,16 @@
         <v>72</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F42" s="2" t="b">
         <v>0</v>
@@ -10264,16 +10314,16 @@
         <v>72</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F43" s="2" t="b">
         <v>0</v>
@@ -10287,7 +10337,9 @@
       <c r="I43" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J43" s="2"/>
+      <c r="J43" s="2">
+        <v>4.0</v>
+      </c>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2" t="b">
@@ -10322,16 +10374,16 @@
         <v>72</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F44" s="2" t="b">
         <v>0</v>
@@ -10345,25 +10397,23 @@
       <c r="I44" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J44" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="K44" s="2">
-        <v>100.0</v>
-      </c>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
       <c r="L44" s="2"/>
       <c r="M44" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="N44" s="2">
-        <v>200.0</v>
-      </c>
+      <c r="N44" s="2"/>
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
-      <c r="S44" s="2"/>
-      <c r="T44" s="2"/>
+      <c r="S44" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T44" s="2">
+        <v>100000.0</v>
+      </c>
       <c r="U44" s="1">
         <v>4.0</v>
       </c>
@@ -10382,16 +10432,16 @@
         <v>72</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>42</v>
+        <v>94</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F45" s="2" t="b">
         <v>0</v>
@@ -10405,29 +10455,23 @@
       <c r="I45" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J45" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="K45" s="2">
-        <v>100.0</v>
-      </c>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="N45" s="2">
-        <v>200.0</v>
-      </c>
+      <c r="N45" s="2"/>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
-      <c r="Q45" s="2"/>
-      <c r="R45" s="2"/>
-      <c r="S45" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="T45" s="2">
-        <v>100000.0</v>
-      </c>
+      <c r="Q45" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="R45" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S45" s="2"/>
+      <c r="T45" s="2"/>
       <c r="U45" s="1">
         <v>4.0</v>
       </c>
@@ -10446,16 +10490,16 @@
         <v>72</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D46" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F46" s="2" t="b">
         <v>0</v>
@@ -10470,18 +10514,16 @@
         <v>0</v>
       </c>
       <c r="J46" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="K46" s="2">
-        <v>100.0</v>
+        <v>150.0</v>
       </c>
       <c r="L46" s="2"/>
       <c r="M46" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="N46" s="2">
-        <v>200.0</v>
-      </c>
+      <c r="N46" s="2"/>
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
@@ -10510,16 +10552,16 @@
         <v>72</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F47" s="2" t="b">
         <v>0</v>
@@ -10533,11 +10575,11 @@
       <c r="I47" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J47" s="2"/>
+      <c r="J47" s="2">
+        <v>4.0</v>
+      </c>
       <c r="K47" s="2"/>
-      <c r="L47" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="L47" s="2"/>
       <c r="M47" s="2" t="b">
         <v>0</v>
       </c>
@@ -10546,8 +10588,12 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
-      <c r="S47" s="2"/>
-      <c r="T47" s="2"/>
+      <c r="S47" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T47" s="2">
+        <v>100000.0</v>
+      </c>
       <c r="U47" s="1">
         <v>4.0</v>
       </c>
@@ -10561,170 +10607,348 @@
       <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
+    <row r="48">
+      <c r="A48" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F48" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I48" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J48" s="2">
+        <v>4.0</v>
+      </c>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
+      <c r="M48" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
-      <c r="S48" s="2"/>
-      <c r="T48" s="2"/>
-      <c r="U48" s="2"/>
+      <c r="S48" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T48" s="2">
+        <v>100000.0</v>
+      </c>
+      <c r="U48" s="1">
+        <v>4.0</v>
+      </c>
       <c r="V48" s="2"/>
-      <c r="W48" s="2"/>
+      <c r="W48" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="X48" s="2"/>
       <c r="Y48" s="2"/>
       <c r="Z48" s="2"/>
       <c r="AA48" s="2"/>
       <c r="AB48" s="2"/>
     </row>
-    <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
+    <row r="49">
+      <c r="A49" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F49" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G49" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H49" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I49" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
+      <c r="M49" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
       <c r="R49" s="2"/>
-      <c r="S49" s="2"/>
-      <c r="T49" s="2"/>
-      <c r="U49" s="2"/>
+      <c r="S49" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T49" s="2">
+        <v>100000.0</v>
+      </c>
+      <c r="U49" s="1">
+        <v>4.0</v>
+      </c>
       <c r="V49" s="2"/>
-      <c r="W49" s="2"/>
+      <c r="W49" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="X49" s="2"/>
       <c r="Y49" s="2"/>
       <c r="Z49" s="2"/>
       <c r="AA49" s="2"/>
       <c r="AB49" s="2"/>
     </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
+    <row r="50">
+      <c r="A50" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F50" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H50" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I50" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J50" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="K50" s="2">
+        <v>100.0</v>
+      </c>
       <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
+      <c r="M50" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N50" s="2">
+        <v>200.0</v>
+      </c>
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
       <c r="S50" s="2"/>
       <c r="T50" s="2"/>
-      <c r="U50" s="2"/>
+      <c r="U50" s="1">
+        <v>4.0</v>
+      </c>
       <c r="V50" s="2"/>
-      <c r="W50" s="2"/>
+      <c r="W50" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="X50" s="2"/>
       <c r="Y50" s="2"/>
       <c r="Z50" s="2"/>
       <c r="AA50" s="2"/>
       <c r="AB50" s="2"/>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
+    <row r="51">
+      <c r="A51" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F51" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G51" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I51" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J51" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="K51" s="2">
+        <v>100.0</v>
+      </c>
       <c r="L51" s="2"/>
-      <c r="M51" s="2"/>
-      <c r="N51" s="2"/>
+      <c r="M51" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N51" s="2">
+        <v>200.0</v>
+      </c>
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
       <c r="R51" s="2"/>
-      <c r="S51" s="2"/>
-      <c r="T51" s="2"/>
-      <c r="U51" s="2"/>
+      <c r="S51" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T51" s="2">
+        <v>100000.0</v>
+      </c>
+      <c r="U51" s="1">
+        <v>4.0</v>
+      </c>
       <c r="V51" s="2"/>
-      <c r="W51" s="2"/>
+      <c r="W51" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="X51" s="2"/>
       <c r="Y51" s="2"/>
       <c r="Z51" s="2"/>
       <c r="AA51" s="2"/>
       <c r="AB51" s="2"/>
     </row>
-    <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
+    <row r="52">
+      <c r="A52" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F52" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G52" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H52" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I52" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J52" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="K52" s="2">
+        <v>100.0</v>
+      </c>
       <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
-      <c r="N52" s="2"/>
+      <c r="M52" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N52" s="2">
+        <v>200.0</v>
+      </c>
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
       <c r="R52" s="2"/>
-      <c r="S52" s="2"/>
-      <c r="T52" s="2"/>
-      <c r="U52" s="2"/>
+      <c r="S52" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T52" s="2">
+        <v>100000.0</v>
+      </c>
+      <c r="U52" s="1">
+        <v>4.0</v>
+      </c>
       <c r="V52" s="2"/>
-      <c r="W52" s="2"/>
+      <c r="W52" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="X52" s="2"/>
       <c r="Y52" s="2"/>
       <c r="Z52" s="2"/>
       <c r="AA52" s="2"/>
       <c r="AB52" s="2"/>
     </row>
-    <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
+    <row r="53">
+      <c r="A53" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F53" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H53" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I53" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
-      <c r="M53" s="2"/>
+      <c r="L53" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M53" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
@@ -10732,9 +10956,13 @@
       <c r="R53" s="2"/>
       <c r="S53" s="2"/>
       <c r="T53" s="2"/>
-      <c r="U53" s="2"/>
+      <c r="U53" s="1">
+        <v>4.0</v>
+      </c>
       <c r="V53" s="2"/>
-      <c r="W53" s="2"/>
+      <c r="W53" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="X53" s="2"/>
       <c r="Y53" s="2"/>
       <c r="Z53" s="2"/>
@@ -15422,40 +15650,184 @@
       <c r="AB209" s="2"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="D210" s="4"/>
-      <c r="O210" s="4"/>
+      <c r="A210" s="2"/>
+      <c r="B210" s="2"/>
+      <c r="C210" s="2"/>
+      <c r="D210" s="2"/>
+      <c r="E210" s="2"/>
+      <c r="F210" s="2"/>
+      <c r="G210" s="2"/>
+      <c r="H210" s="2"/>
+      <c r="I210" s="2"/>
+      <c r="J210" s="2"/>
+      <c r="K210" s="2"/>
+      <c r="L210" s="2"/>
+      <c r="M210" s="2"/>
+      <c r="N210" s="2"/>
+      <c r="O210" s="2"/>
       <c r="P210" s="2"/>
-      <c r="Q210" s="4"/>
+      <c r="Q210" s="2"/>
+      <c r="R210" s="2"/>
+      <c r="S210" s="2"/>
+      <c r="T210" s="2"/>
+      <c r="U210" s="2"/>
+      <c r="V210" s="2"/>
+      <c r="W210" s="2"/>
+      <c r="X210" s="2"/>
+      <c r="Y210" s="2"/>
+      <c r="Z210" s="2"/>
+      <c r="AA210" s="2"/>
+      <c r="AB210" s="2"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="D211" s="4"/>
-      <c r="O211" s="4"/>
+      <c r="A211" s="2"/>
+      <c r="B211" s="2"/>
+      <c r="C211" s="2"/>
+      <c r="D211" s="2"/>
+      <c r="E211" s="2"/>
+      <c r="F211" s="2"/>
+      <c r="G211" s="2"/>
+      <c r="H211" s="2"/>
+      <c r="I211" s="2"/>
+      <c r="J211" s="2"/>
+      <c r="K211" s="2"/>
+      <c r="L211" s="2"/>
+      <c r="M211" s="2"/>
+      <c r="N211" s="2"/>
+      <c r="O211" s="2"/>
       <c r="P211" s="2"/>
-      <c r="Q211" s="4"/>
+      <c r="Q211" s="2"/>
+      <c r="R211" s="2"/>
+      <c r="S211" s="2"/>
+      <c r="T211" s="2"/>
+      <c r="U211" s="2"/>
+      <c r="V211" s="2"/>
+      <c r="W211" s="2"/>
+      <c r="X211" s="2"/>
+      <c r="Y211" s="2"/>
+      <c r="Z211" s="2"/>
+      <c r="AA211" s="2"/>
+      <c r="AB211" s="2"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="D212" s="4"/>
-      <c r="O212" s="4"/>
+      <c r="A212" s="2"/>
+      <c r="B212" s="2"/>
+      <c r="C212" s="2"/>
+      <c r="D212" s="2"/>
+      <c r="E212" s="2"/>
+      <c r="F212" s="2"/>
+      <c r="G212" s="2"/>
+      <c r="H212" s="2"/>
+      <c r="I212" s="2"/>
+      <c r="J212" s="2"/>
+      <c r="K212" s="2"/>
+      <c r="L212" s="2"/>
+      <c r="M212" s="2"/>
+      <c r="N212" s="2"/>
+      <c r="O212" s="2"/>
       <c r="P212" s="2"/>
-      <c r="Q212" s="4"/>
+      <c r="Q212" s="2"/>
+      <c r="R212" s="2"/>
+      <c r="S212" s="2"/>
+      <c r="T212" s="2"/>
+      <c r="U212" s="2"/>
+      <c r="V212" s="2"/>
+      <c r="W212" s="2"/>
+      <c r="X212" s="2"/>
+      <c r="Y212" s="2"/>
+      <c r="Z212" s="2"/>
+      <c r="AA212" s="2"/>
+      <c r="AB212" s="2"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="D213" s="4"/>
-      <c r="O213" s="4"/>
+      <c r="A213" s="2"/>
+      <c r="B213" s="2"/>
+      <c r="C213" s="2"/>
+      <c r="D213" s="2"/>
+      <c r="E213" s="2"/>
+      <c r="F213" s="2"/>
+      <c r="G213" s="2"/>
+      <c r="H213" s="2"/>
+      <c r="I213" s="2"/>
+      <c r="J213" s="2"/>
+      <c r="K213" s="2"/>
+      <c r="L213" s="2"/>
+      <c r="M213" s="2"/>
+      <c r="N213" s="2"/>
+      <c r="O213" s="2"/>
       <c r="P213" s="2"/>
-      <c r="Q213" s="4"/>
+      <c r="Q213" s="2"/>
+      <c r="R213" s="2"/>
+      <c r="S213" s="2"/>
+      <c r="T213" s="2"/>
+      <c r="U213" s="2"/>
+      <c r="V213" s="2"/>
+      <c r="W213" s="2"/>
+      <c r="X213" s="2"/>
+      <c r="Y213" s="2"/>
+      <c r="Z213" s="2"/>
+      <c r="AA213" s="2"/>
+      <c r="AB213" s="2"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="D214" s="4"/>
-      <c r="O214" s="4"/>
+      <c r="A214" s="2"/>
+      <c r="B214" s="2"/>
+      <c r="C214" s="2"/>
+      <c r="D214" s="2"/>
+      <c r="E214" s="2"/>
+      <c r="F214" s="2"/>
+      <c r="G214" s="2"/>
+      <c r="H214" s="2"/>
+      <c r="I214" s="2"/>
+      <c r="J214" s="2"/>
+      <c r="K214" s="2"/>
+      <c r="L214" s="2"/>
+      <c r="M214" s="2"/>
+      <c r="N214" s="2"/>
+      <c r="O214" s="2"/>
       <c r="P214" s="2"/>
-      <c r="Q214" s="4"/>
+      <c r="Q214" s="2"/>
+      <c r="R214" s="2"/>
+      <c r="S214" s="2"/>
+      <c r="T214" s="2"/>
+      <c r="U214" s="2"/>
+      <c r="V214" s="2"/>
+      <c r="W214" s="2"/>
+      <c r="X214" s="2"/>
+      <c r="Y214" s="2"/>
+      <c r="Z214" s="2"/>
+      <c r="AA214" s="2"/>
+      <c r="AB214" s="2"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="D215" s="4"/>
-      <c r="O215" s="4"/>
+      <c r="A215" s="2"/>
+      <c r="B215" s="2"/>
+      <c r="C215" s="2"/>
+      <c r="D215" s="2"/>
+      <c r="E215" s="2"/>
+      <c r="F215" s="2"/>
+      <c r="G215" s="2"/>
+      <c r="H215" s="2"/>
+      <c r="I215" s="2"/>
+      <c r="J215" s="2"/>
+      <c r="K215" s="2"/>
+      <c r="L215" s="2"/>
+      <c r="M215" s="2"/>
+      <c r="N215" s="2"/>
+      <c r="O215" s="2"/>
       <c r="P215" s="2"/>
-      <c r="Q215" s="4"/>
+      <c r="Q215" s="2"/>
+      <c r="R215" s="2"/>
+      <c r="S215" s="2"/>
+      <c r="T215" s="2"/>
+      <c r="U215" s="2"/>
+      <c r="V215" s="2"/>
+      <c r="W215" s="2"/>
+      <c r="X215" s="2"/>
+      <c r="Y215" s="2"/>
+      <c r="Z215" s="2"/>
+      <c r="AA215" s="2"/>
+      <c r="AB215" s="2"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
       <c r="D216" s="4"/>
@@ -20059,18 +20431,54 @@
       <c r="P982" s="2"/>
       <c r="Q982" s="4"/>
     </row>
+    <row r="983" ht="15.75" customHeight="1">
+      <c r="D983" s="4"/>
+      <c r="O983" s="4"/>
+      <c r="P983" s="2"/>
+      <c r="Q983" s="4"/>
+    </row>
+    <row r="984" ht="15.75" customHeight="1">
+      <c r="D984" s="4"/>
+      <c r="O984" s="4"/>
+      <c r="P984" s="2"/>
+      <c r="Q984" s="4"/>
+    </row>
+    <row r="985" ht="15.75" customHeight="1">
+      <c r="D985" s="4"/>
+      <c r="O985" s="4"/>
+      <c r="P985" s="2"/>
+      <c r="Q985" s="4"/>
+    </row>
+    <row r="986" ht="15.75" customHeight="1">
+      <c r="D986" s="4"/>
+      <c r="O986" s="4"/>
+      <c r="P986" s="2"/>
+      <c r="Q986" s="4"/>
+    </row>
+    <row r="987" ht="15.75" customHeight="1">
+      <c r="D987" s="4"/>
+      <c r="O987" s="4"/>
+      <c r="P987" s="2"/>
+      <c r="Q987" s="4"/>
+    </row>
+    <row r="988" ht="15.75" customHeight="1">
+      <c r="D988" s="4"/>
+      <c r="O988" s="4"/>
+      <c r="P988" s="2"/>
+      <c r="Q988" s="4"/>
+    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="Q2:Q982">
+    <dataValidation type="list" allowBlank="1" sqref="Q2:Q988">
       <formula1>"UserLocal,DateOnly,TimeZoneIndependent"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="O2:O982">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="O2:O988">
       <formula1>"Text,TextArea,Email,Url,TickerSymbol,Phone"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="D2:D982">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="D2:D988">
       <formula1>"Boolean,Date,Decimal,Double,Integer,Lookup,Money,Picklist,String,Memo,Status"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="P2:P982">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="P2:P988">
       <formula1>"None,Duration,Language,TimeZone"</formula1>
     </dataValidation>
   </dataValidations>
@@ -20106,16 +20514,16 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="2"/>
@@ -20141,7 +20549,7 @@
     <row r="2">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>0</v>
@@ -20150,7 +20558,7 @@
         <v>1.0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -20176,7 +20584,7 @@
     <row r="3">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>0</v>
@@ -20185,7 +20593,7 @@
         <v>2.0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -20210,10 +20618,10 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
@@ -20222,7 +20630,7 @@
         <v>1.0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -20247,10 +20655,10 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
@@ -20259,7 +20667,7 @@
         <v>2.0</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -20285,7 +20693,7 @@
     <row r="6">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>0</v>
@@ -20294,7 +20702,7 @@
         <v>1.0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -20321,7 +20729,7 @@
     <row r="7">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>0</v>
@@ -20330,7 +20738,7 @@
         <v>2.0</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -26915,37 +27323,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -26965,7 +27373,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>12</v>
@@ -26986,16 +27394,16 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="J2" s="2">
         <v>15000.0</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -27015,7 +27423,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
@@ -27036,13 +27444,13 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="K3" s="2">
         <v>20000.0</v>

</xml_diff>

<commit_message>
Order within calculate plugin where dependencies
</commit_message>
<xml_diff>
--- a/Customisations/Test Customisations Calculations.xlsx
+++ b/Customisations/Test Customisations Calculations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="142">
   <si>
     <t>Display Name</t>
   </si>
@@ -257,6 +257,33 @@
   </si>
   <si>
     <t>jmcg_dateaddresultnotimezone</t>
+  </si>
+  <si>
+    <t>jmcg_timetakenstartutc</t>
+  </si>
+  <si>
+    <t>jmcg_timetakenendutc</t>
+  </si>
+  <si>
+    <t>jmcg_timetakenutc</t>
+  </si>
+  <si>
+    <t>jmcg_timetakenstartdateonly</t>
+  </si>
+  <si>
+    <t>jmcg_timetakenenddateonly</t>
+  </si>
+  <si>
+    <t>jmcg_timetakendateonly</t>
+  </si>
+  <si>
+    <t>jmcg_timetakenstartnotimezone</t>
+  </si>
+  <si>
+    <t>jmcg_timetakenendnotimezone</t>
+  </si>
+  <si>
+    <t>jmcg_timetakennotimezone</t>
   </si>
   <si>
     <t>jmcg_integersumsource</t>
@@ -9373,7 +9400,9 @@
       <c r="Q27" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="R27" s="2"/>
+      <c r="R27" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="S27" s="2">
         <v>0.0</v>
       </c>
@@ -9651,7 +9680,7 @@
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>81</v>
@@ -9659,8 +9688,8 @@
       <c r="C32" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>42</v>
+      <c r="D32" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>81</v>
@@ -9690,7 +9719,9 @@
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
+      <c r="Q32" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="R32" s="2"/>
       <c r="S32" s="2">
         <v>0.0</v>
@@ -9713,7 +9744,7 @@
     </row>
     <row r="33">
       <c r="A33" s="3" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>82</v>
@@ -9721,8 +9752,8 @@
       <c r="C33" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>44</v>
+      <c r="D33" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>82</v>
@@ -9740,9 +9771,11 @@
         <v>0</v>
       </c>
       <c r="J33" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="K33" s="2"/>
+        <v>3.0</v>
+      </c>
+      <c r="K33" s="2">
+        <v>150.0</v>
+      </c>
       <c r="L33" s="2"/>
       <c r="M33" s="2" t="b">
         <v>0</v>
@@ -9750,7 +9783,9 @@
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
-      <c r="Q33" s="2"/>
+      <c r="Q33" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="R33" s="2"/>
       <c r="S33" s="2">
         <v>0.0</v>
@@ -9773,7 +9808,7 @@
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>83</v>
@@ -9781,8 +9816,8 @@
       <c r="C34" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>46</v>
+      <c r="D34" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>83</v>
@@ -9800,9 +9835,11 @@
         <v>0</v>
       </c>
       <c r="J34" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="K34" s="2"/>
+        <v>3.0</v>
+      </c>
+      <c r="K34" s="2">
+        <v>150.0</v>
+      </c>
       <c r="L34" s="2"/>
       <c r="M34" s="2" t="b">
         <v>0</v>
@@ -9810,7 +9847,9 @@
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
-      <c r="Q34" s="2"/>
+      <c r="Q34" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="R34" s="2"/>
       <c r="S34" s="2">
         <v>0.0</v>
@@ -9833,7 +9872,7 @@
     </row>
     <row r="35">
       <c r="A35" s="3" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>84</v>
@@ -9841,8 +9880,8 @@
       <c r="C35" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>48</v>
+      <c r="D35" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>84</v>
@@ -9859,8 +9898,12 @@
       <c r="I35" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
+      <c r="J35" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="K35" s="2">
+        <v>150.0</v>
+      </c>
       <c r="L35" s="2"/>
       <c r="M35" s="2" t="b">
         <v>0</v>
@@ -9868,7 +9911,9 @@
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
-      <c r="Q35" s="2"/>
+      <c r="Q35" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="R35" s="2"/>
       <c r="S35" s="2">
         <v>0.0</v>
@@ -9891,7 +9936,7 @@
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>85</v>
@@ -9899,8 +9944,8 @@
       <c r="C36" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>42</v>
+      <c r="D36" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>85</v>
@@ -9930,7 +9975,9 @@
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
-      <c r="Q36" s="2"/>
+      <c r="Q36" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="R36" s="2"/>
       <c r="S36" s="2">
         <v>0.0</v>
@@ -9953,7 +10000,7 @@
     </row>
     <row r="37">
       <c r="A37" s="3" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>86</v>
@@ -9961,8 +10008,8 @@
       <c r="C37" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>44</v>
+      <c r="D37" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>86</v>
@@ -9980,9 +10027,11 @@
         <v>0</v>
       </c>
       <c r="J37" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="K37" s="2"/>
+        <v>3.0</v>
+      </c>
+      <c r="K37" s="2">
+        <v>150.0</v>
+      </c>
       <c r="L37" s="2"/>
       <c r="M37" s="2" t="b">
         <v>0</v>
@@ -9990,7 +10039,9 @@
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
-      <c r="Q37" s="2"/>
+      <c r="Q37" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="R37" s="2"/>
       <c r="S37" s="2">
         <v>0.0</v>
@@ -10013,7 +10064,7 @@
     </row>
     <row r="38">
       <c r="A38" s="3" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>87</v>
@@ -10021,8 +10072,8 @@
       <c r="C38" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>46</v>
+      <c r="D38" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>87</v>
@@ -10040,9 +10091,11 @@
         <v>0</v>
       </c>
       <c r="J38" s="2">
-        <v>4.0</v>
-      </c>
-      <c r="K38" s="2"/>
+        <v>3.0</v>
+      </c>
+      <c r="K38" s="2">
+        <v>150.0</v>
+      </c>
       <c r="L38" s="2"/>
       <c r="M38" s="2" t="b">
         <v>0</v>
@@ -10050,7 +10103,9 @@
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
-      <c r="Q38" s="2"/>
+      <c r="Q38" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="R38" s="2"/>
       <c r="S38" s="2">
         <v>0.0</v>
@@ -10073,7 +10128,7 @@
     </row>
     <row r="39">
       <c r="A39" s="3" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>88</v>
@@ -10081,8 +10136,8 @@
       <c r="C39" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>48</v>
+      <c r="D39" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>88</v>
@@ -10099,8 +10154,12 @@
       <c r="I39" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
+      <c r="J39" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="K39" s="2">
+        <v>150.0</v>
+      </c>
       <c r="L39" s="2"/>
       <c r="M39" s="2" t="b">
         <v>0</v>
@@ -10108,7 +10167,9 @@
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
+      <c r="Q39" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="R39" s="2"/>
       <c r="S39" s="2">
         <v>0.0</v>
@@ -10131,7 +10192,7 @@
     </row>
     <row r="40">
       <c r="A40" s="3" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>89</v>
@@ -10139,8 +10200,8 @@
       <c r="C40" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>54</v>
+      <c r="D40" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>89</v>
@@ -10157,8 +10218,12 @@
       <c r="I40" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
+      <c r="J40" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="K40" s="2">
+        <v>150.0</v>
+      </c>
       <c r="L40" s="2"/>
       <c r="M40" s="2" t="b">
         <v>0</v>
@@ -10166,14 +10231,16 @@
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
-      <c r="Q40" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="R40" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="S40" s="2"/>
-      <c r="T40" s="2"/>
+      <c r="Q40" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T40" s="2">
+        <v>100000.0</v>
+      </c>
       <c r="U40" s="1">
         <v>4.0</v>
       </c>
@@ -10438,7 +10505,7 @@
         <v>94</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>94</v>
@@ -10455,8 +10522,12 @@
       <c r="I45" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
+      <c r="J45" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="K45" s="2">
+        <v>150.0</v>
+      </c>
       <c r="L45" s="2"/>
       <c r="M45" s="2" t="b">
         <v>0</v>
@@ -10464,14 +10535,14 @@
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
-      <c r="Q45" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="R45" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="S45" s="2"/>
-      <c r="T45" s="2"/>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="2"/>
+      <c r="S45" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T45" s="2">
+        <v>100000.0</v>
+      </c>
       <c r="U45" s="1">
         <v>4.0</v>
       </c>
@@ -10496,7 +10567,7 @@
         <v>95</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>95</v>
@@ -10514,11 +10585,9 @@
         <v>0</v>
       </c>
       <c r="J46" s="2">
-        <v>3.0</v>
-      </c>
-      <c r="K46" s="2">
-        <v>150.0</v>
-      </c>
+        <v>4.0</v>
+      </c>
+      <c r="K46" s="2"/>
       <c r="L46" s="2"/>
       <c r="M46" s="2" t="b">
         <v>0</v>
@@ -10558,7 +10627,7 @@
         <v>96</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>96</v>
@@ -10618,7 +10687,7 @@
         <v>97</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>97</v>
@@ -10635,9 +10704,7 @@
       <c r="I48" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J48" s="2">
-        <v>4.0</v>
-      </c>
+      <c r="J48" s="2"/>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
       <c r="M48" s="2" t="b">
@@ -10678,7 +10745,7 @@
         <v>98</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>98</v>
@@ -10704,14 +10771,14 @@
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
-      <c r="Q49" s="2"/>
-      <c r="R49" s="2"/>
-      <c r="S49" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="T49" s="2">
-        <v>100000.0</v>
-      </c>
+      <c r="Q49" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="R49" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S49" s="2"/>
+      <c r="T49" s="2"/>
       <c r="U49" s="1">
         <v>4.0</v>
       </c>
@@ -10736,7 +10803,7 @@
         <v>99</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>100</v>
+        <v>42</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>99</v>
@@ -10754,24 +10821,26 @@
         <v>0</v>
       </c>
       <c r="J50" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="K50" s="2">
-        <v>100.0</v>
+        <v>150.0</v>
       </c>
       <c r="L50" s="2"/>
       <c r="M50" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="N50" s="2">
-        <v>200.0</v>
-      </c>
+      <c r="N50" s="2"/>
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
-      <c r="S50" s="2"/>
-      <c r="T50" s="2"/>
+      <c r="S50" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T50" s="2">
+        <v>100000.0</v>
+      </c>
       <c r="U50" s="1">
         <v>4.0</v>
       </c>
@@ -10790,16 +10859,16 @@
         <v>72</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>42</v>
+        <v>100</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F51" s="2" t="b">
         <v>0</v>
@@ -10814,18 +10883,14 @@
         <v>0</v>
       </c>
       <c r="J51" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="K51" s="2">
-        <v>100.0</v>
-      </c>
+        <v>4.0</v>
+      </c>
+      <c r="K51" s="2"/>
       <c r="L51" s="2"/>
       <c r="M51" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="N51" s="2">
-        <v>200.0</v>
-      </c>
+      <c r="N51" s="2"/>
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
@@ -10854,16 +10919,16 @@
         <v>72</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>42</v>
+        <v>101</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F52" s="2" t="b">
         <v>0</v>
@@ -10878,18 +10943,14 @@
         <v>0</v>
       </c>
       <c r="J52" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="K52" s="2">
-        <v>100.0</v>
-      </c>
+        <v>4.0</v>
+      </c>
+      <c r="K52" s="2"/>
       <c r="L52" s="2"/>
       <c r="M52" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="N52" s="2">
-        <v>200.0</v>
-      </c>
+      <c r="N52" s="2"/>
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
@@ -10918,16 +10979,16 @@
         <v>72</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F53" s="2" t="b">
         <v>0</v>
@@ -10943,9 +11004,7 @@
       </c>
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
-      <c r="L53" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="L53" s="2"/>
       <c r="M53" s="2" t="b">
         <v>0</v>
       </c>
@@ -10954,8 +11013,12 @@
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
-      <c r="S53" s="2"/>
-      <c r="T53" s="2"/>
+      <c r="S53" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T53" s="2">
+        <v>100000.0</v>
+      </c>
       <c r="U53" s="1">
         <v>4.0</v>
       </c>
@@ -10969,260 +11032,528 @@
       <c r="AA53" s="2"/>
       <c r="AB53" s="2"/>
     </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
+    <row r="54">
+      <c r="A54" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F54" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G54" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H54" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I54" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
-      <c r="M54" s="2"/>
+      <c r="M54" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
-      <c r="Q54" s="2"/>
-      <c r="R54" s="2"/>
+      <c r="Q54" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="R54" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="S54" s="2"/>
       <c r="T54" s="2"/>
-      <c r="U54" s="2"/>
+      <c r="U54" s="1">
+        <v>4.0</v>
+      </c>
       <c r="V54" s="2"/>
-      <c r="W54" s="2"/>
+      <c r="W54" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="X54" s="2"/>
       <c r="Y54" s="2"/>
       <c r="Z54" s="2"/>
       <c r="AA54" s="2"/>
       <c r="AB54" s="2"/>
     </row>
-    <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
+    <row r="55">
+      <c r="A55" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F55" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H55" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I55" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J55" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="K55" s="2">
+        <v>150.0</v>
+      </c>
       <c r="L55" s="2"/>
-      <c r="M55" s="2"/>
+      <c r="M55" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
-      <c r="S55" s="2"/>
-      <c r="T55" s="2"/>
-      <c r="U55" s="2"/>
+      <c r="S55" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T55" s="2">
+        <v>100000.0</v>
+      </c>
+      <c r="U55" s="1">
+        <v>4.0</v>
+      </c>
       <c r="V55" s="2"/>
-      <c r="W55" s="2"/>
+      <c r="W55" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="X55" s="2"/>
       <c r="Y55" s="2"/>
       <c r="Z55" s="2"/>
       <c r="AA55" s="2"/>
       <c r="AB55" s="2"/>
     </row>
-    <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
+    <row r="56">
+      <c r="A56" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F56" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G56" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H56" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I56" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J56" s="2">
+        <v>4.0</v>
+      </c>
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
-      <c r="M56" s="2"/>
+      <c r="M56" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
       <c r="R56" s="2"/>
-      <c r="S56" s="2"/>
-      <c r="T56" s="2"/>
-      <c r="U56" s="2"/>
+      <c r="S56" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T56" s="2">
+        <v>100000.0</v>
+      </c>
+      <c r="U56" s="1">
+        <v>4.0</v>
+      </c>
       <c r="V56" s="2"/>
-      <c r="W56" s="2"/>
+      <c r="W56" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="X56" s="2"/>
       <c r="Y56" s="2"/>
       <c r="Z56" s="2"/>
       <c r="AA56" s="2"/>
       <c r="AB56" s="2"/>
     </row>
-    <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
+    <row r="57">
+      <c r="A57" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F57" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G57" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H57" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I57" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J57" s="2">
+        <v>4.0</v>
+      </c>
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
-      <c r="M57" s="2"/>
+      <c r="M57" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
       <c r="P57" s="2"/>
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
-      <c r="S57" s="2"/>
-      <c r="T57" s="2"/>
-      <c r="U57" s="2"/>
+      <c r="S57" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T57" s="2">
+        <v>100000.0</v>
+      </c>
+      <c r="U57" s="1">
+        <v>4.0</v>
+      </c>
       <c r="V57" s="2"/>
-      <c r="W57" s="2"/>
+      <c r="W57" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="X57" s="2"/>
       <c r="Y57" s="2"/>
       <c r="Z57" s="2"/>
       <c r="AA57" s="2"/>
       <c r="AB57" s="2"/>
     </row>
-    <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
+    <row r="58">
+      <c r="A58" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F58" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G58" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H58" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I58" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
-      <c r="M58" s="2"/>
+      <c r="M58" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="N58" s="2"/>
       <c r="O58" s="2"/>
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
       <c r="R58" s="2"/>
-      <c r="S58" s="2"/>
-      <c r="T58" s="2"/>
-      <c r="U58" s="2"/>
+      <c r="S58" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T58" s="2">
+        <v>100000.0</v>
+      </c>
+      <c r="U58" s="1">
+        <v>4.0</v>
+      </c>
       <c r="V58" s="2"/>
-      <c r="W58" s="2"/>
+      <c r="W58" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="X58" s="2"/>
       <c r="Y58" s="2"/>
       <c r="Z58" s="2"/>
       <c r="AA58" s="2"/>
       <c r="AB58" s="2"/>
     </row>
-    <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
+    <row r="59">
+      <c r="A59" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F59" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G59" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H59" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I59" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J59" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="K59" s="2">
+        <v>100.0</v>
+      </c>
       <c r="L59" s="2"/>
-      <c r="M59" s="2"/>
-      <c r="N59" s="2"/>
+      <c r="M59" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N59" s="2">
+        <v>200.0</v>
+      </c>
       <c r="O59" s="2"/>
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
       <c r="R59" s="2"/>
       <c r="S59" s="2"/>
       <c r="T59" s="2"/>
-      <c r="U59" s="2"/>
+      <c r="U59" s="1">
+        <v>4.0</v>
+      </c>
       <c r="V59" s="2"/>
-      <c r="W59" s="2"/>
+      <c r="W59" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="X59" s="2"/>
       <c r="Y59" s="2"/>
       <c r="Z59" s="2"/>
       <c r="AA59" s="2"/>
       <c r="AB59" s="2"/>
     </row>
-    <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
-      <c r="K60" s="2"/>
+    <row r="60">
+      <c r="A60" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F60" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G60" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H60" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I60" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J60" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="K60" s="2">
+        <v>100.0</v>
+      </c>
       <c r="L60" s="2"/>
-      <c r="M60" s="2"/>
-      <c r="N60" s="2"/>
+      <c r="M60" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N60" s="2">
+        <v>200.0</v>
+      </c>
       <c r="O60" s="2"/>
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
-      <c r="S60" s="2"/>
-      <c r="T60" s="2"/>
-      <c r="U60" s="2"/>
+      <c r="S60" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T60" s="2">
+        <v>100000.0</v>
+      </c>
+      <c r="U60" s="1">
+        <v>4.0</v>
+      </c>
       <c r="V60" s="2"/>
-      <c r="W60" s="2"/>
+      <c r="W60" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="X60" s="2"/>
       <c r="Y60" s="2"/>
       <c r="Z60" s="2"/>
       <c r="AA60" s="2"/>
       <c r="AB60" s="2"/>
     </row>
-    <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
+    <row r="61">
+      <c r="A61" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F61" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G61" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H61" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I61" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J61" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="K61" s="2">
+        <v>100.0</v>
+      </c>
       <c r="L61" s="2"/>
-      <c r="M61" s="2"/>
-      <c r="N61" s="2"/>
+      <c r="M61" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N61" s="2">
+        <v>200.0</v>
+      </c>
       <c r="O61" s="2"/>
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
-      <c r="S61" s="2"/>
-      <c r="T61" s="2"/>
-      <c r="U61" s="2"/>
+      <c r="S61" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="T61" s="2">
+        <v>100000.0</v>
+      </c>
+      <c r="U61" s="1">
+        <v>4.0</v>
+      </c>
       <c r="V61" s="2"/>
-      <c r="W61" s="2"/>
+      <c r="W61" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="X61" s="2"/>
       <c r="Y61" s="2"/>
       <c r="Z61" s="2"/>
       <c r="AA61" s="2"/>
       <c r="AB61" s="2"/>
     </row>
-    <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
+    <row r="62">
+      <c r="A62" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F62" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G62" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H62" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I62" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
-      <c r="M62" s="2"/>
+      <c r="L62" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M62" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="N62" s="2"/>
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
@@ -11230,9 +11561,13 @@
       <c r="R62" s="2"/>
       <c r="S62" s="2"/>
       <c r="T62" s="2"/>
-      <c r="U62" s="2"/>
+      <c r="U62" s="1">
+        <v>4.0</v>
+      </c>
       <c r="V62" s="2"/>
-      <c r="W62" s="2"/>
+      <c r="W62" s="2" t="b">
+        <v>0</v>
+      </c>
       <c r="X62" s="2"/>
       <c r="Y62" s="2"/>
       <c r="Z62" s="2"/>
@@ -15830,58 +16165,274 @@
       <c r="AB215" s="2"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="D216" s="4"/>
-      <c r="O216" s="4"/>
+      <c r="A216" s="2"/>
+      <c r="B216" s="2"/>
+      <c r="C216" s="2"/>
+      <c r="D216" s="2"/>
+      <c r="E216" s="2"/>
+      <c r="F216" s="2"/>
+      <c r="G216" s="2"/>
+      <c r="H216" s="2"/>
+      <c r="I216" s="2"/>
+      <c r="J216" s="2"/>
+      <c r="K216" s="2"/>
+      <c r="L216" s="2"/>
+      <c r="M216" s="2"/>
+      <c r="N216" s="2"/>
+      <c r="O216" s="2"/>
       <c r="P216" s="2"/>
-      <c r="Q216" s="4"/>
+      <c r="Q216" s="2"/>
+      <c r="R216" s="2"/>
+      <c r="S216" s="2"/>
+      <c r="T216" s="2"/>
+      <c r="U216" s="2"/>
+      <c r="V216" s="2"/>
+      <c r="W216" s="2"/>
+      <c r="X216" s="2"/>
+      <c r="Y216" s="2"/>
+      <c r="Z216" s="2"/>
+      <c r="AA216" s="2"/>
+      <c r="AB216" s="2"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="D217" s="4"/>
-      <c r="O217" s="4"/>
+      <c r="A217" s="2"/>
+      <c r="B217" s="2"/>
+      <c r="C217" s="2"/>
+      <c r="D217" s="2"/>
+      <c r="E217" s="2"/>
+      <c r="F217" s="2"/>
+      <c r="G217" s="2"/>
+      <c r="H217" s="2"/>
+      <c r="I217" s="2"/>
+      <c r="J217" s="2"/>
+      <c r="K217" s="2"/>
+      <c r="L217" s="2"/>
+      <c r="M217" s="2"/>
+      <c r="N217" s="2"/>
+      <c r="O217" s="2"/>
       <c r="P217" s="2"/>
-      <c r="Q217" s="4"/>
+      <c r="Q217" s="2"/>
+      <c r="R217" s="2"/>
+      <c r="S217" s="2"/>
+      <c r="T217" s="2"/>
+      <c r="U217" s="2"/>
+      <c r="V217" s="2"/>
+      <c r="W217" s="2"/>
+      <c r="X217" s="2"/>
+      <c r="Y217" s="2"/>
+      <c r="Z217" s="2"/>
+      <c r="AA217" s="2"/>
+      <c r="AB217" s="2"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="D218" s="4"/>
-      <c r="O218" s="4"/>
+      <c r="A218" s="2"/>
+      <c r="B218" s="2"/>
+      <c r="C218" s="2"/>
+      <c r="D218" s="2"/>
+      <c r="E218" s="2"/>
+      <c r="F218" s="2"/>
+      <c r="G218" s="2"/>
+      <c r="H218" s="2"/>
+      <c r="I218" s="2"/>
+      <c r="J218" s="2"/>
+      <c r="K218" s="2"/>
+      <c r="L218" s="2"/>
+      <c r="M218" s="2"/>
+      <c r="N218" s="2"/>
+      <c r="O218" s="2"/>
       <c r="P218" s="2"/>
-      <c r="Q218" s="4"/>
+      <c r="Q218" s="2"/>
+      <c r="R218" s="2"/>
+      <c r="S218" s="2"/>
+      <c r="T218" s="2"/>
+      <c r="U218" s="2"/>
+      <c r="V218" s="2"/>
+      <c r="W218" s="2"/>
+      <c r="X218" s="2"/>
+      <c r="Y218" s="2"/>
+      <c r="Z218" s="2"/>
+      <c r="AA218" s="2"/>
+      <c r="AB218" s="2"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="D219" s="4"/>
-      <c r="O219" s="4"/>
+      <c r="A219" s="2"/>
+      <c r="B219" s="2"/>
+      <c r="C219" s="2"/>
+      <c r="D219" s="2"/>
+      <c r="E219" s="2"/>
+      <c r="F219" s="2"/>
+      <c r="G219" s="2"/>
+      <c r="H219" s="2"/>
+      <c r="I219" s="2"/>
+      <c r="J219" s="2"/>
+      <c r="K219" s="2"/>
+      <c r="L219" s="2"/>
+      <c r="M219" s="2"/>
+      <c r="N219" s="2"/>
+      <c r="O219" s="2"/>
       <c r="P219" s="2"/>
-      <c r="Q219" s="4"/>
+      <c r="Q219" s="2"/>
+      <c r="R219" s="2"/>
+      <c r="S219" s="2"/>
+      <c r="T219" s="2"/>
+      <c r="U219" s="2"/>
+      <c r="V219" s="2"/>
+      <c r="W219" s="2"/>
+      <c r="X219" s="2"/>
+      <c r="Y219" s="2"/>
+      <c r="Z219" s="2"/>
+      <c r="AA219" s="2"/>
+      <c r="AB219" s="2"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="D220" s="4"/>
-      <c r="O220" s="4"/>
+      <c r="A220" s="2"/>
+      <c r="B220" s="2"/>
+      <c r="C220" s="2"/>
+      <c r="D220" s="2"/>
+      <c r="E220" s="2"/>
+      <c r="F220" s="2"/>
+      <c r="G220" s="2"/>
+      <c r="H220" s="2"/>
+      <c r="I220" s="2"/>
+      <c r="J220" s="2"/>
+      <c r="K220" s="2"/>
+      <c r="L220" s="2"/>
+      <c r="M220" s="2"/>
+      <c r="N220" s="2"/>
+      <c r="O220" s="2"/>
       <c r="P220" s="2"/>
-      <c r="Q220" s="4"/>
+      <c r="Q220" s="2"/>
+      <c r="R220" s="2"/>
+      <c r="S220" s="2"/>
+      <c r="T220" s="2"/>
+      <c r="U220" s="2"/>
+      <c r="V220" s="2"/>
+      <c r="W220" s="2"/>
+      <c r="X220" s="2"/>
+      <c r="Y220" s="2"/>
+      <c r="Z220" s="2"/>
+      <c r="AA220" s="2"/>
+      <c r="AB220" s="2"/>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="D221" s="4"/>
-      <c r="O221" s="4"/>
+      <c r="A221" s="2"/>
+      <c r="B221" s="2"/>
+      <c r="C221" s="2"/>
+      <c r="D221" s="2"/>
+      <c r="E221" s="2"/>
+      <c r="F221" s="2"/>
+      <c r="G221" s="2"/>
+      <c r="H221" s="2"/>
+      <c r="I221" s="2"/>
+      <c r="J221" s="2"/>
+      <c r="K221" s="2"/>
+      <c r="L221" s="2"/>
+      <c r="M221" s="2"/>
+      <c r="N221" s="2"/>
+      <c r="O221" s="2"/>
       <c r="P221" s="2"/>
-      <c r="Q221" s="4"/>
+      <c r="Q221" s="2"/>
+      <c r="R221" s="2"/>
+      <c r="S221" s="2"/>
+      <c r="T221" s="2"/>
+      <c r="U221" s="2"/>
+      <c r="V221" s="2"/>
+      <c r="W221" s="2"/>
+      <c r="X221" s="2"/>
+      <c r="Y221" s="2"/>
+      <c r="Z221" s="2"/>
+      <c r="AA221" s="2"/>
+      <c r="AB221" s="2"/>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="D222" s="4"/>
-      <c r="O222" s="4"/>
+      <c r="A222" s="2"/>
+      <c r="B222" s="2"/>
+      <c r="C222" s="2"/>
+      <c r="D222" s="2"/>
+      <c r="E222" s="2"/>
+      <c r="F222" s="2"/>
+      <c r="G222" s="2"/>
+      <c r="H222" s="2"/>
+      <c r="I222" s="2"/>
+      <c r="J222" s="2"/>
+      <c r="K222" s="2"/>
+      <c r="L222" s="2"/>
+      <c r="M222" s="2"/>
+      <c r="N222" s="2"/>
+      <c r="O222" s="2"/>
       <c r="P222" s="2"/>
-      <c r="Q222" s="4"/>
+      <c r="Q222" s="2"/>
+      <c r="R222" s="2"/>
+      <c r="S222" s="2"/>
+      <c r="T222" s="2"/>
+      <c r="U222" s="2"/>
+      <c r="V222" s="2"/>
+      <c r="W222" s="2"/>
+      <c r="X222" s="2"/>
+      <c r="Y222" s="2"/>
+      <c r="Z222" s="2"/>
+      <c r="AA222" s="2"/>
+      <c r="AB222" s="2"/>
     </row>
     <row r="223" ht="15.75" customHeight="1">
-      <c r="D223" s="4"/>
-      <c r="O223" s="4"/>
+      <c r="A223" s="2"/>
+      <c r="B223" s="2"/>
+      <c r="C223" s="2"/>
+      <c r="D223" s="2"/>
+      <c r="E223" s="2"/>
+      <c r="F223" s="2"/>
+      <c r="G223" s="2"/>
+      <c r="H223" s="2"/>
+      <c r="I223" s="2"/>
+      <c r="J223" s="2"/>
+      <c r="K223" s="2"/>
+      <c r="L223" s="2"/>
+      <c r="M223" s="2"/>
+      <c r="N223" s="2"/>
+      <c r="O223" s="2"/>
       <c r="P223" s="2"/>
-      <c r="Q223" s="4"/>
+      <c r="Q223" s="2"/>
+      <c r="R223" s="2"/>
+      <c r="S223" s="2"/>
+      <c r="T223" s="2"/>
+      <c r="U223" s="2"/>
+      <c r="V223" s="2"/>
+      <c r="W223" s="2"/>
+      <c r="X223" s="2"/>
+      <c r="Y223" s="2"/>
+      <c r="Z223" s="2"/>
+      <c r="AA223" s="2"/>
+      <c r="AB223" s="2"/>
     </row>
     <row r="224" ht="15.75" customHeight="1">
-      <c r="D224" s="4"/>
-      <c r="O224" s="4"/>
+      <c r="A224" s="2"/>
+      <c r="B224" s="2"/>
+      <c r="C224" s="2"/>
+      <c r="D224" s="2"/>
+      <c r="E224" s="2"/>
+      <c r="F224" s="2"/>
+      <c r="G224" s="2"/>
+      <c r="H224" s="2"/>
+      <c r="I224" s="2"/>
+      <c r="J224" s="2"/>
+      <c r="K224" s="2"/>
+      <c r="L224" s="2"/>
+      <c r="M224" s="2"/>
+      <c r="N224" s="2"/>
+      <c r="O224" s="2"/>
       <c r="P224" s="2"/>
-      <c r="Q224" s="4"/>
+      <c r="Q224" s="2"/>
+      <c r="R224" s="2"/>
+      <c r="S224" s="2"/>
+      <c r="T224" s="2"/>
+      <c r="U224" s="2"/>
+      <c r="V224" s="2"/>
+      <c r="W224" s="2"/>
+      <c r="X224" s="2"/>
+      <c r="Y224" s="2"/>
+      <c r="Z224" s="2"/>
+      <c r="AA224" s="2"/>
+      <c r="AB224" s="2"/>
     </row>
     <row r="225" ht="15.75" customHeight="1">
       <c r="D225" s="4"/>
@@ -20467,18 +21018,72 @@
       <c r="P988" s="2"/>
       <c r="Q988" s="4"/>
     </row>
+    <row r="989" ht="15.75" customHeight="1">
+      <c r="D989" s="4"/>
+      <c r="O989" s="4"/>
+      <c r="P989" s="2"/>
+      <c r="Q989" s="4"/>
+    </row>
+    <row r="990" ht="15.75" customHeight="1">
+      <c r="D990" s="4"/>
+      <c r="O990" s="4"/>
+      <c r="P990" s="2"/>
+      <c r="Q990" s="4"/>
+    </row>
+    <row r="991" ht="15.75" customHeight="1">
+      <c r="D991" s="4"/>
+      <c r="O991" s="4"/>
+      <c r="P991" s="2"/>
+      <c r="Q991" s="4"/>
+    </row>
+    <row r="992" ht="15.75" customHeight="1">
+      <c r="D992" s="4"/>
+      <c r="O992" s="4"/>
+      <c r="P992" s="2"/>
+      <c r="Q992" s="4"/>
+    </row>
+    <row r="993" ht="15.75" customHeight="1">
+      <c r="D993" s="4"/>
+      <c r="O993" s="4"/>
+      <c r="P993" s="2"/>
+      <c r="Q993" s="4"/>
+    </row>
+    <row r="994" ht="15.75" customHeight="1">
+      <c r="D994" s="4"/>
+      <c r="O994" s="4"/>
+      <c r="P994" s="2"/>
+      <c r="Q994" s="4"/>
+    </row>
+    <row r="995" ht="15.75" customHeight="1">
+      <c r="D995" s="4"/>
+      <c r="O995" s="4"/>
+      <c r="P995" s="2"/>
+      <c r="Q995" s="4"/>
+    </row>
+    <row r="996" ht="15.75" customHeight="1">
+      <c r="D996" s="4"/>
+      <c r="O996" s="4"/>
+      <c r="P996" s="2"/>
+      <c r="Q996" s="4"/>
+    </row>
+    <row r="997" ht="15.75" customHeight="1">
+      <c r="D997" s="4"/>
+      <c r="O997" s="4"/>
+      <c r="P997" s="2"/>
+      <c r="Q997" s="4"/>
+    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="Q2:Q988">
+    <dataValidation type="list" allowBlank="1" sqref="Q2:Q997">
       <formula1>"UserLocal,DateOnly,TimeZoneIndependent"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="O2:O988">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="O2:O997">
       <formula1>"Text,TextArea,Email,Url,TickerSymbol,Phone"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="D2:D988">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="D2:D997">
       <formula1>"Boolean,Date,Decimal,Double,Integer,Lookup,Money,Picklist,String,Memo,Status"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="P2:P988">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="P2:P997">
       <formula1>"None,Duration,Language,TimeZone"</formula1>
     </dataValidation>
   </dataValidations>
@@ -20514,16 +21119,16 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="2"/>
@@ -20549,7 +21154,7 @@
     <row r="2">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>0</v>
@@ -20558,7 +21163,7 @@
         <v>1.0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -20584,7 +21189,7 @@
     <row r="3">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>0</v>
@@ -20593,7 +21198,7 @@
         <v>2.0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -20618,10 +21223,10 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
@@ -20630,7 +21235,7 @@
         <v>1.0</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -20655,10 +21260,10 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
@@ -20667,7 +21272,7 @@
         <v>2.0</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -20693,7 +21298,7 @@
     <row r="6">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>0</v>
@@ -20702,7 +21307,7 @@
         <v>1.0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -20729,7 +21334,7 @@
     <row r="7">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>0</v>
@@ -20738,7 +21343,7 @@
         <v>2.0</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -27323,37 +27928,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -27373,7 +27978,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>12</v>
@@ -27394,16 +27999,16 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="J2" s="2">
         <v>15000.0</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -27423,7 +28028,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
@@ -27444,13 +28049,13 @@
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="K3" s="2">
         <v>20000.0</v>

</xml_diff>